<commit_message>
LBCB 1 & 2 shunt calibrations
</commit_message>
<xml_diff>
--- a/Config/Calibrations/Crane Bay ShuntCal LBCB1.xlsx
+++ b/Config/Calibrations/Crane Bay ShuntCal LBCB1.xlsx
@@ -726,13 +726,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.0895100000000002</c:v>
+                  <c:v>3.02902</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.187671</c:v>
+                  <c:v>0.12922600000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.70695</c:v>
+                  <c:v>-2.76335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,11 +765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150541376"/>
-        <c:axId val="150541952"/>
+        <c:axId val="85581120"/>
+        <c:axId val="93364224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150541376"/>
+        <c:axId val="85581120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,12 +843,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150541952"/>
+        <c:crossAx val="93364224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150541952"/>
+        <c:axId val="93364224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,7 +932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150541376"/>
+        <c:crossAx val="85581120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1177,13 +1177,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.95716</c:v>
+                  <c:v>2.9851299999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2485500000000003E-2</c:v>
+                  <c:v>0.11280800000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.7913999999999999</c:v>
+                  <c:v>-2.7593399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,11 +1216,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99841088"/>
-        <c:axId val="99841664"/>
+        <c:axId val="93365952"/>
+        <c:axId val="93366528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99841088"/>
+        <c:axId val="93365952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,12 +1294,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99841664"/>
+        <c:crossAx val="93366528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99841664"/>
+        <c:axId val="93366528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99841088"/>
+        <c:crossAx val="93365952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1628,13 +1628,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.0139</c:v>
+                  <c:v>2.9815900000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12667400000000001</c:v>
+                  <c:v>9.8238000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.74499</c:v>
+                  <c:v>-2.76844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1667,11 +1667,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="140578176"/>
-        <c:axId val="140581056"/>
+        <c:axId val="93368256"/>
+        <c:axId val="93368832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140578176"/>
+        <c:axId val="93368256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,12 +1745,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140581056"/>
+        <c:crossAx val="93368832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140581056"/>
+        <c:axId val="93368832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140578176"/>
+        <c:crossAx val="93368256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2079,13 +2079,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.6030099999999998</c:v>
+                  <c:v>3.4376099999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66711399999999998</c:v>
+                  <c:v>0.50129900000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.27033</c:v>
+                  <c:v>-2.4350800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2118,11 +2118,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142053312"/>
-        <c:axId val="142053888"/>
+        <c:axId val="93370560"/>
+        <c:axId val="93371136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142053312"/>
+        <c:axId val="93370560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,12 +2196,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142053888"/>
+        <c:crossAx val="93371136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142053888"/>
+        <c:axId val="93371136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2285,7 +2285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142053312"/>
+        <c:crossAx val="93370560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2530,13 +2530,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.8841999999999999</c:v>
+                  <c:v>3.1833999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.35252E-2</c:v>
+                  <c:v>0.277055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.9273799999999999</c:v>
+                  <c:v>-2.62683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2569,11 +2569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142075008"/>
-        <c:axId val="150537344"/>
+        <c:axId val="100147776"/>
+        <c:axId val="100148352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142075008"/>
+        <c:axId val="100147776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2647,12 +2647,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150537344"/>
+        <c:crossAx val="100148352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150537344"/>
+        <c:axId val="100148352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2736,7 +2736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142075008"/>
+        <c:crossAx val="100147776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2981,13 +2981,13 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.98366</c:v>
+                  <c:v>3.2374200000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9250800000000001E-2</c:v>
+                  <c:v>0.32539499999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.8436699999999999</c:v>
+                  <c:v>-2.5872000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3020,11 +3020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142079616"/>
-        <c:axId val="150538496"/>
+        <c:axId val="100150080"/>
+        <c:axId val="100150656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142079616"/>
+        <c:axId val="100150080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3098,12 +3098,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150538496"/>
+        <c:crossAx val="100150656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150538496"/>
+        <c:axId val="100150656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3187,7 +3187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142079616"/>
+        <c:crossAx val="100150080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3794,74 +3794,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="58" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>32.806390958932603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>33.309124132459601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="60" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>33.366599678886999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="60" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>32.637019618164203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="60" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>32.982133385550199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="61" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="62" t="s">
         <v>47</v>
+      </c>
+      <c r="C8">
+        <v>32.800186152233898</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
@@ -3897,7 +3915,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4470,7 +4488,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5">
-        <v>3.0895100000000002</v>
+        <v>3.02902</v>
       </c>
       <c r="C40" s="4">
         <f>B33</f>
@@ -4490,7 +4508,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>0.187671</v>
+        <v>0.12922600000000001</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -4507,7 +4525,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5">
-        <v>-2.70695</v>
+        <v>-2.76335</v>
       </c>
       <c r="C42" s="4">
         <f>B35</f>
@@ -4528,7 +4546,7 @@
       </c>
       <c r="M45" s="1">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>32.783242625724228</v>
+        <v>32.806390958932568</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -4537,7 +4555,7 @@
       </c>
       <c r="M46" s="1">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99998914082152979</v>
+        <v>0.9999891441669666</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -4546,7 +4564,7 @@
       </c>
       <c r="M47" s="1">
         <f>330/M45</f>
-        <v>10.066118344896635</v>
+        <v>10.059015647685779</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -4555,7 +4573,7 @@
       </c>
       <c r="M48" s="1">
         <f>-(-10-B41)*M45</f>
-        <v>333.98489018405456</v>
+        <v>332.30334826738465</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -4564,7 +4582,7 @@
       </c>
       <c r="M49" s="1">
         <f>-(10-B41)*M45</f>
-        <v>-321.67996233042999</v>
+        <v>-323.8244709112667</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -4588,7 +4606,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5161,7 +5179,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5">
-        <v>2.95716</v>
+        <v>2.9851299999999998</v>
       </c>
       <c r="C40" s="4">
         <f>B33</f>
@@ -5181,7 +5199,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>8.2485500000000003E-2</v>
+        <v>0.11280800000000001</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -5198,7 +5216,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5">
-        <v>-2.7913999999999999</v>
+        <v>-2.7593399999999999</v>
       </c>
       <c r="C42" s="4">
         <f>B35</f>
@@ -5219,7 +5237,7 @@
       </c>
       <c r="M45" s="1">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>33.285425312186668</v>
+        <v>33.309124132459566</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -5228,7 +5246,7 @@
       </c>
       <c r="M46" s="1">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999999865050926</v>
+        <v>0.99999999029975495</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -5237,7 +5255,7 @@
       </c>
       <c r="M47" s="1">
         <f>330/M45</f>
-        <v>9.9142491617548405</v>
+        <v>9.9071953584758692</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -5246,7 +5264,7 @@
       </c>
       <c r="M48" s="1">
         <f>-(-10-B41)*M45</f>
-        <v>335.59981807145505</v>
+        <v>336.84877699973015</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -5255,7 +5273,7 @@
       </c>
       <c r="M49" s="1">
         <f>-(10-B41)*M45</f>
-        <v>-330.10868817227828</v>
+        <v>-329.33370564946119</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -5279,7 +5297,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5852,7 +5870,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5">
-        <v>3.0139</v>
+        <v>2.9815900000000002</v>
       </c>
       <c r="C40" s="4">
         <f>B33</f>
@@ -5872,7 +5890,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>0.12667400000000001</v>
+        <v>9.8238000000000006E-2</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -5889,7 +5907,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5">
-        <v>-2.74499</v>
+        <v>-2.76844</v>
       </c>
       <c r="C42" s="4">
         <f>B35</f>
@@ -5910,7 +5928,7 @@
       </c>
       <c r="M45" s="1">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>33.315267474546495</v>
+        <v>33.366599678886992</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -5919,7 +5937,7 @@
       </c>
       <c r="M46" s="1">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999868628452759</v>
+        <v>0.99999893473505452</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -5928,7 +5946,7 @@
       </c>
       <c r="M47" s="1">
         <f>330/M45</f>
-        <v>9.9053684696401234</v>
+        <v>9.8901297457891815</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -5937,7 +5955,7 @@
       </c>
       <c r="M48" s="1">
         <f>-(-10-B41)*M45</f>
-        <v>337.37285293753564</v>
+        <v>336.94386480812443</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -5946,7 +5964,7 @@
       </c>
       <c r="M49" s="1">
         <f>-(10-B41)*M45</f>
-        <v>-328.93249655339429</v>
+        <v>-330.38812876961543</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -5970,7 +5988,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6543,7 +6561,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5">
-        <v>3.6030099999999998</v>
+        <v>3.4376099999999998</v>
       </c>
       <c r="C40" s="4">
         <f>B33</f>
@@ -6563,7 +6581,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>0.66711399999999998</v>
+        <v>0.50129900000000005</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -6580,7 +6598,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5">
-        <v>-2.27033</v>
+        <v>-2.4350800000000001</v>
       </c>
       <c r="C42" s="4">
         <f>B35</f>
@@ -6601,7 +6619,7 @@
       </c>
       <c r="M45" s="1">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>32.633409822087813</v>
+        <v>32.637019618164224</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -6610,7 +6628,7 @@
       </c>
       <c r="M46" s="1">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999979290738816</v>
+        <v>0.99999963933036484</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -6619,7 +6637,7 @@
       </c>
       <c r="M47" s="1">
         <f>330/M45</f>
-        <v>10.112335848417551</v>
+        <v>10.111217380165975</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -6628,7 +6646,7 @@
       </c>
       <c r="M48" s="1">
         <f>-(-10-B41)*M45</f>
-        <v>348.10430278093042</v>
+        <v>342.73110147920835</v>
       </c>
     </row>
     <row r="49" spans="12:13" x14ac:dyDescent="0.2">
@@ -6637,7 +6655,7 @@
       </c>
       <c r="M49" s="1">
         <f>-(10-B41)*M45</f>
-        <v>-304.56389366082584</v>
+        <v>-310.00929088407617</v>
       </c>
     </row>
     <row r="51" spans="12:13" x14ac:dyDescent="0.2">
@@ -6661,7 +6679,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView topLeftCell="A27" zoomScale="85" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7234,7 +7252,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5">
-        <v>2.8841999999999999</v>
+        <v>3.1833999999999998</v>
       </c>
       <c r="C40" s="4">
         <f>B33</f>
@@ -7254,7 +7272,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>-2.35252E-2</v>
+        <v>0.277055</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -7271,7 +7289,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5">
-        <v>-2.9273799999999999</v>
+        <v>-2.62683</v>
       </c>
       <c r="C42" s="4">
         <f>B35</f>
@@ -7292,7 +7310,7 @@
       </c>
       <c r="M45" s="1">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>32.97447029119953</v>
+        <v>32.982133385550185</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -7301,7 +7319,7 @@
       </c>
       <c r="M46" s="1">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999999300450182</v>
+        <v>0.99999999681678187</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -7310,7 +7328,7 @@
       </c>
       <c r="M47" s="1">
         <f>330/M45</f>
-        <v>10.007742265023522</v>
+        <v>10.005417058454334</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -7319,7 +7337,7 @@
       </c>
       <c r="M48" s="1">
         <f>-(-10-B41)*M45</f>
-        <v>328.9689719035008</v>
+        <v>338.95919882063549</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -7328,7 +7346,7 @@
       </c>
       <c r="M49" s="1">
         <f>-(10-B41)*M45</f>
-        <v>-330.52043392048984</v>
+        <v>-320.6834688903682</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -7347,7 +7365,7 @@
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="54">
         <f>B41</f>
-        <v>-2.35252E-2</v>
+        <v>0.277055</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -7368,7 +7386,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7941,7 +7959,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5">
-        <v>2.98366</v>
+        <v>3.2374200000000002</v>
       </c>
       <c r="C40" s="4">
         <f>B33</f>
@@ -7961,7 +7979,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>6.9250800000000001E-2</v>
+        <v>0.32539499999999999</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -7978,7 +7996,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5">
-        <v>-2.8436699999999999</v>
+        <v>-2.5872000000000002</v>
       </c>
       <c r="C42" s="4">
         <f>B35</f>
@@ -7999,7 +8017,7 @@
       </c>
       <c r="M45" s="1">
         <f>SLOPE(C40:C42,B40:B42)</f>
-        <v>32.784913512551327</v>
+        <v>32.800186152233948</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -8008,7 +8026,7 @@
       </c>
       <c r="M46" s="1">
         <f>RSQ(C40:C42,B40:B42)</f>
-        <v>0.99999167858980553</v>
+        <v>0.99999281373316318</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -8017,7 +8035,7 @@
       </c>
       <c r="M47" s="1">
         <f>330/M45</f>
-        <v>10.065605324036108</v>
+        <v>10.060918510290968</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -8026,7 +8044,7 @@
       </c>
       <c r="M48" s="1">
         <f>-(-10-B41)*M45</f>
-        <v>330.11951661418829</v>
+        <v>338.67487809534566</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -8035,7 +8053,7 @@
       </c>
       <c r="M49" s="1">
         <f>-(10-B41)*M45</f>
-        <v>-325.57875363683826</v>
+        <v>-317.3288449493333</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -8046,7 +8064,7 @@
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="54">
         <f>B41</f>
-        <v>6.9250800000000001E-2</v>
+        <v>0.32539499999999999</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>48</v>

</xml_diff>